<commit_message>
Add shacdn, add print all page, add options
</commit_message>
<xml_diff>
--- a/db/panne.xlsx
+++ b/db/panne.xlsx
@@ -9,8 +9,9 @@
   </bookViews>
   <sheets>
     <sheet name="Vector" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="MK ULTRA BOOM DAAM LE BOIS" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="AQUI" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Scie" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Plaqueuse" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Stockeur" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t xml:space="preserve">Date de début</t>
   </si>
@@ -48,34 +49,55 @@
     <t xml:space="preserve">Vector</t>
   </si>
   <si>
-    <t xml:space="preserve">Changement outil meche de 3</t>
+    <t xml:space="preserve">Changement meche de 3</t>
   </si>
   <si>
     <t xml:space="preserve">Changement outil fraise à rainurer</t>
   </si>
   <si>
+    <t xml:space="preserve">Changement meche de 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changement meche de 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scie</t>
+  </si>
+  <si>
     <t xml:space="preserve">Graissage</t>
   </si>
   <si>
-    <t xml:space="preserve">Daam les petites</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MK ULTRA BOOM DAAM LE BOIS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Changement de mistinguette</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WOAF WOAF </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mmmhhhh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aqui vieux ben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AQUI 2000</t>
+    <t xml:space="preserve">Changement lame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plaqueuse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opé 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stockeur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opé 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opé 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opé 4</t>
   </si>
 </sst>
 </file>
@@ -86,8 +108,8 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="h:mm;@"/>
-    <numFmt numFmtId="167" formatCode="hh:mm"/>
-    <numFmt numFmtId="168" formatCode="[$-F800]dddd&quot;, &quot;mmmm\ dd&quot;, &quot;yyyy"/>
+    <numFmt numFmtId="167" formatCode="[$-F800]dddd&quot;, &quot;mmmm\ dd&quot;, &quot;yyyy"/>
+    <numFmt numFmtId="168" formatCode="hh:mm"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -163,27 +185,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -218,7 +240,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E5" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E6" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:E6"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Date de début"/>
+    <tableColumn id="2" name="Heure"/>
+    <tableColumn id="3" name="Durée"/>
+    <tableColumn id="4" name="Récurrence en jours"/>
+    <tableColumn id="5" name="Opération"/>
+  </tableColumns>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau1_2" displayName="Tableau1_2" ref="A1:E4" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:E4"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Date de début"/>
+    <tableColumn id="2" name="Heure"/>
+    <tableColumn id="3" name="Durée"/>
+    <tableColumn id="4" name="Récurrence en jours"/>
+    <tableColumn id="5" name="Opération"/>
+  </tableColumns>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau1_3" displayName="Tableau1_3" ref="A1:E5" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A1:E5"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date de début"/>
@@ -230,21 +278,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau1_2" displayName="Tableau1_2" ref="A1:E7" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:E7"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Date de début"/>
-    <tableColumn id="2" name="Heure"/>
-    <tableColumn id="3" name="Durée"/>
-    <tableColumn id="4" name="Récurrence en jours"/>
-    <tableColumn id="5" name="Opération"/>
-  </tableColumns>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau1_3" displayName="Tableau1_3" ref="A1:E5" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau1_35" displayName="Tableau1_35" ref="A1:E5" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A1:E5"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date de début"/>
@@ -433,116 +468,180 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1048576"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="25.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.56"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
         <v>45310</v>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="3" t="n">
         <v>0.4375</v>
       </c>
-      <c r="C2" s="5" t="n">
+      <c r="C2" s="3" t="n">
         <v>0.0625</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="0" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>45315</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
+        <v>45308</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>45306</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
         <v>45307</v>
       </c>
-      <c r="B3" s="4" t="n">
+      <c r="B6" s="3" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C3" s="5" t="n">
-        <v>0.0208333333333333</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
-        <v>45308</v>
-      </c>
-      <c r="B4" s="4" t="n">
-        <v>0.458333333333333</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>0.0208333333333333</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
-        <v>45309</v>
-      </c>
-      <c r="B5" s="4" t="n">
-        <v>0.458333333333333</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>0.0208333333333333</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C6" s="3" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -565,119 +664,107 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="25.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="33.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="33.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>45309</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>0.4375</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>45308</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
         <v>45306</v>
       </c>
-      <c r="B2" s="4" t="n">
-        <v>0.583333333333333</v>
-      </c>
-      <c r="C2" s="5" t="n">
-        <v>0.0625</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
-        <v>45306</v>
-      </c>
-      <c r="B3" s="4" t="n">
-        <v>0.666666666666667</v>
-      </c>
-      <c r="C3" s="5" t="n">
-        <v>0.0208333333333333</v>
-      </c>
-      <c r="D3" s="1" t="n">
+      <c r="B4" s="3" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
-        <v>45308</v>
-      </c>
-      <c r="B4" s="4" t="n">
-        <v>0.583333333333333</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>0.0208333333333333</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
-        <v>45307</v>
-      </c>
-      <c r="B5" s="4" t="n">
-        <v>0.583333333333333</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>0.0208333333333333</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -698,115 +785,239 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1048576"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="25.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="33.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="33.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
         <v>45310</v>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="3" t="n">
         <v>0.4375</v>
       </c>
-      <c r="C2" s="5" t="n">
+      <c r="C2" s="6" t="n">
         <v>0.0625</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>45307</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="D3" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="1" t="s">
+      <c r="E3" s="0" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
+        <v>45308</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>45309</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <tableParts>
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="33.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>45310</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>0.4375</v>
+      </c>
+      <c r="C2" s="6" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
         <v>45307</v>
       </c>
-      <c r="B3" s="4" t="n">
+      <c r="B3" s="3" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C3" s="5" t="n">
-        <v>0.0208333333333333</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+      <c r="C3" s="6" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
         <v>45308</v>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="3" t="n">
         <v>0.666666666666667</v>
       </c>
-      <c r="C4" s="5" t="n">
-        <v>0.0208333333333333</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+      <c r="C4" s="6" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
         <v>45309</v>
       </c>
-      <c r="B5" s="4" t="n">
+      <c r="B5" s="3" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="C5" s="5" t="n">
-        <v>0.0208333333333333</v>
-      </c>
-      <c r="D5" s="1" t="n">
+      <c r="C5" s="6" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="D5" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="E5" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>